<commit_message>
updating feedback forms and trying to resolve new error/warnings
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/dairy_digester_operator_feedback_v005.xlsx
+++ b/feedback_forms/current_versions/dairy_digester_operator_feedback_v005.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117C9928-9E91-43FC-935D-2B0B214E1B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB31801-DD57-4FF2-ACFD-45F737648F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4333" yWindow="1073" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="3993" yWindow="733" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -3641,7 +3641,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -8506,15 +8508,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
@@ -8523,6 +8516,15 @@
     <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8761,20 +8763,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
     <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>